<commit_message>
first stage of the data corrections
</commit_message>
<xml_diff>
--- a/indicators/output/classified_indicators.xlsx
+++ b/indicators/output/classified_indicators.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,11 +491,6 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Commune</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
           <t>Indicator Type</t>
         </is>
       </c>
@@ -531,7 +526,6 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -564,7 +558,6 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -614,8 +607,7 @@
       <c r="K4" t="n">
         <v>75</v>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Evaluation Indicator</t>
         </is>
@@ -669,8 +661,7 @@
       <c r="K5" t="n">
         <v>92</v>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -724,8 +715,7 @@
       <c r="K6" t="n">
         <v>36</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -779,8 +769,7 @@
       <c r="K7" t="n">
         <v>5</v>
       </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -834,8 +823,7 @@
       <c r="K8" t="n">
         <v>93</v>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -889,8 +877,7 @@
       <c r="K9" t="n">
         <v>15</v>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -944,8 +931,7 @@
       <c r="K10" t="n">
         <v>6</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -999,8 +985,7 @@
       <c r="K11" t="n">
         <v>38</v>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1054,8 +1039,7 @@
       <c r="K12" t="n">
         <v>38</v>
       </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>Evaluation Indicator</t>
         </is>
@@ -1109,8 +1093,7 @@
       <c r="K13" t="n">
         <v>5</v>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1164,8 +1147,7 @@
       <c r="K14" t="n">
         <v>4</v>
       </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1219,8 +1201,7 @@
       <c r="K15" t="n">
         <v>92</v>
       </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>Evaluation Indicator</t>
         </is>
@@ -1274,8 +1255,7 @@
       <c r="K16" t="n">
         <v>50</v>
       </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1329,8 +1309,7 @@
       <c r="K17" t="n">
         <v>41</v>
       </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1384,8 +1363,7 @@
       <c r="K18" t="n">
         <v>2</v>
       </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1439,8 +1417,7 @@
       <c r="K19" t="n">
         <v>100</v>
       </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1494,8 +1471,7 @@
       <c r="K20" t="n">
         <v>18</v>
       </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1532,7 +1508,6 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1582,8 +1557,7 @@
       <c r="K22" t="n">
         <v>72</v>
       </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1637,8 +1611,7 @@
       <c r="K23" t="n">
         <v>76</v>
       </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>Evaluation Indicator</t>
         </is>
@@ -1692,8 +1665,7 @@
       <c r="K24" t="n">
         <v>97</v>
       </c>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1747,8 +1719,7 @@
       <c r="K25" t="n">
         <v>95</v>
       </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1802,8 +1773,7 @@
       <c r="K26" t="n">
         <v>1929</v>
       </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1857,8 +1827,7 @@
       <c r="K27" t="n">
         <v>11</v>
       </c>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1912,8 +1881,7 @@
       <c r="K28" t="n">
         <v>119</v>
       </c>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr">
+      <c r="L28" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -1963,8 +1931,7 @@
       <c r="K29" t="n">
         <v>54.5</v>
       </c>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2018,8 +1985,7 @@
       <c r="K30" t="n">
         <v>1958</v>
       </c>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr">
+      <c r="L30" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2073,8 +2039,7 @@
       <c r="K31" t="n">
         <v>2</v>
       </c>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr">
+      <c r="L31" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2128,8 +2093,7 @@
       <c r="K32" t="n">
         <v>2</v>
       </c>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2183,8 +2147,7 @@
       <c r="K33" t="n">
         <v>96</v>
       </c>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr">
+      <c r="L33" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2238,8 +2201,7 @@
       <c r="K34" t="n">
         <v>88</v>
       </c>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr">
+      <c r="L34" t="inlineStr">
         <is>
           <t>Evaluation Indicator</t>
         </is>
@@ -2293,8 +2255,7 @@
       <c r="K35" t="n">
         <v>73</v>
       </c>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr">
+      <c r="L35" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2348,8 +2309,7 @@
       <c r="K36" t="n">
         <v>1055</v>
       </c>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr">
+      <c r="L36" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2403,8 +2363,7 @@
       <c r="K37" t="n">
         <v>117</v>
       </c>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr">
+      <c r="L37" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2458,8 +2417,7 @@
       <c r="K38" t="n">
         <v>134</v>
       </c>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr">
+      <c r="L38" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2513,8 +2471,7 @@
       <c r="K39" t="n">
         <v>43</v>
       </c>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr">
+      <c r="L39" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2568,8 +2525,7 @@
       <c r="K40" t="n">
         <v>91</v>
       </c>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr">
+      <c r="L40" t="inlineStr">
         <is>
           <t>Evaluation Indicator</t>
         </is>
@@ -2623,8 +2579,7 @@
       <c r="K41" t="n">
         <v>85</v>
       </c>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr">
+      <c r="L41" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2678,8 +2633,7 @@
       <c r="K42" t="n">
         <v>48</v>
       </c>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr">
+      <c r="L42" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2733,8 +2687,7 @@
       <c r="K43" t="n">
         <v>61</v>
       </c>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr">
+      <c r="L43" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2788,8 +2741,7 @@
       <c r="K44" t="n">
         <v>8</v>
       </c>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr">
+      <c r="L44" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2843,8 +2795,7 @@
       <c r="K45" t="n">
         <v>68</v>
       </c>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr">
+      <c r="L45" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2898,8 +2849,7 @@
       <c r="K46" t="n">
         <v>100</v>
       </c>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr">
+      <c r="L46" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -2953,8 +2903,7 @@
       <c r="K47" t="n">
         <v>135</v>
       </c>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr">
+      <c r="L47" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3008,8 +2957,7 @@
       <c r="K48" t="n">
         <v>11</v>
       </c>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr">
+      <c r="L48" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3063,8 +3011,7 @@
       <c r="K49" t="n">
         <v>146</v>
       </c>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr">
+      <c r="L49" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3118,8 +3065,7 @@
       <c r="K50" t="n">
         <v>96</v>
       </c>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr">
+      <c r="L50" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3173,8 +3119,7 @@
       <c r="K51" t="n">
         <v>164</v>
       </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr">
+      <c r="L51" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3228,8 +3173,7 @@
       <c r="K52" t="n">
         <v>160</v>
       </c>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr">
+      <c r="L52" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3266,7 +3210,6 @@
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3314,8 +3257,7 @@
       <c r="K54" t="n">
         <v>1590019</v>
       </c>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr">
+      <c r="L54" t="inlineStr">
         <is>
           <t>Evaluation Indicator</t>
         </is>
@@ -3369,8 +3311,7 @@
       <c r="K55" t="n">
         <v>85</v>
       </c>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr">
+      <c r="L55" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3424,8 +3365,7 @@
       <c r="K56" t="n">
         <v>6714</v>
       </c>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr">
+      <c r="L56" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3479,8 +3419,7 @@
       <c r="K57" t="n">
         <v>16246</v>
       </c>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr">
+      <c r="L57" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3534,8 +3473,7 @@
       <c r="K58" t="n">
         <v>61</v>
       </c>
-      <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr">
+      <c r="L58" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3589,8 +3527,7 @@
       <c r="K59" t="n">
         <v>2</v>
       </c>
-      <c r="L59" t="inlineStr"/>
-      <c r="M59" t="inlineStr">
+      <c r="L59" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>
@@ -3644,8 +3581,7 @@
       <c r="K60" t="n">
         <v>54</v>
       </c>
-      <c r="L60" t="inlineStr"/>
-      <c r="M60" t="inlineStr">
+      <c r="L60" t="inlineStr">
         <is>
           <t>Monitoring Indicator</t>
         </is>

</xml_diff>